<commit_message>
2. Scraping Best10 Reviews & ratings
</commit_message>
<xml_diff>
--- a/results/baby_bed_All.xlsx
+++ b/results/baby_bed_All.xlsx
@@ -9,7 +9,6 @@
   <sheets>
     <sheet name="Raw" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="V2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="best10" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -4255,6 +4254,8 @@
 View 139 reviews about Portable. 96% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
           <t xml:space="preserve">Portable </t>
@@ -4298,6 +4299,8 @@
 View 85 reviews about Craftsmanship. 58% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
           <t xml:space="preserve">Craftsmanship </t>
@@ -4341,6 +4344,8 @@
 View 77 reviews about Comfort. 64% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
           <t xml:space="preserve">Comfort </t>
@@ -4384,6 +4389,8 @@
 View 47 reviews about Good sound quality. 68% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr">
         <is>
           <t xml:space="preserve">Good sound quality </t>
@@ -4427,6 +4434,8 @@
 View 63 reviews about Ample storage. 95% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr">
         <is>
           <t xml:space="preserve">Ample storage </t>
@@ -4470,6 +4479,8 @@
 View 57 reviews about Calming. 90% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr">
         <is>
           <t xml:space="preserve">Calming </t>
@@ -4513,6 +4524,8 @@
 View 12 reviews about Easy to clean. 86% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr">
         <is>
           <t xml:space="preserve">Easy to clean </t>
@@ -4556,6 +4569,8 @@
 View 8 reviews about Ease of use. 88% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
           <t xml:space="preserve">Ease of use </t>
@@ -4599,6 +4614,8 @@
 View 5 reviews about Safety measures. 60% of the reviews are negative.</t>
         </is>
       </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
           <t xml:space="preserve">Safety measures </t>
@@ -4801,6 +4818,8 @@
 View 112 reviews about Craftsmanship. 54% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr">
         <is>
           <t xml:space="preserve">Craftsmanship </t>
@@ -4844,6 +4863,8 @@
 View 57 reviews about Durability. 53% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr">
         <is>
           <t xml:space="preserve">Durability </t>
@@ -4887,6 +4908,8 @@
 View 20 reviews about Compact. 100% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr">
         <is>
           <t xml:space="preserve">Compact </t>
@@ -4930,6 +4953,8 @@
 View 9 reviews about Safety measures. 89% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr">
         <is>
           <t xml:space="preserve">Safety measures </t>
@@ -4973,6 +4998,8 @@
 View 6 reviews about Odor. 67% of the reviews are negative.</t>
         </is>
       </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr">
         <is>
           <t xml:space="preserve">Odor </t>
@@ -5175,6 +5202,8 @@
 View 289 reviews about Well made. 78% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr">
         <is>
           <t xml:space="preserve">Well made </t>
@@ -5218,6 +5247,8 @@
 View 142 reviews about Lacks durability. 67% of the reviews are negative.</t>
         </is>
       </c>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr">
         <is>
           <t xml:space="preserve">Lacks durability </t>
@@ -5261,6 +5292,8 @@
 View 98 reviews about Compact. 88% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr">
         <is>
           <t xml:space="preserve">Compact </t>
@@ -5304,6 +5337,8 @@
 View 12 reviews about Unpleasant odor. 67% of the reviews are negative.</t>
         </is>
       </c>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr">
         <is>
           <t xml:space="preserve">Unpleasant odor </t>
@@ -5347,6 +5382,8 @@
 View 5 reviews about Safety measures. 100% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr">
         <is>
           <t xml:space="preserve">Safety measures </t>
@@ -5549,6 +5586,8 @@
 View 94 reviews about Well made. 87% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
       <c r="I33" t="inlineStr">
         <is>
           <t xml:space="preserve">Well made </t>
@@ -5592,6 +5631,8 @@
 View 41 reviews about Durability. 61% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
       <c r="I34" t="inlineStr">
         <is>
           <t xml:space="preserve">Durability </t>
@@ -5635,6 +5676,8 @@
 View 25 reviews about Compact. 96% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
       <c r="I35" t="inlineStr">
         <is>
           <t xml:space="preserve">Compact </t>
@@ -5678,6 +5721,8 @@
 View 13 reviews about Unpleasant odor. 76% of the reviews are negative.</t>
         </is>
       </c>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
       <c r="I36" t="inlineStr">
         <is>
           <t xml:space="preserve">Unpleasant odor </t>
@@ -5721,6 +5766,8 @@
 View 3 reviews about Safety measures. 67% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr">
         <is>
           <t xml:space="preserve">Safety measures </t>
@@ -5923,6 +5970,8 @@
 View 112 reviews about Craftsmanship. 54% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr">
         <is>
           <t xml:space="preserve">Craftsmanship </t>
@@ -5966,6 +6015,8 @@
 View 57 reviews about Durability. 53% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
       <c r="I42" t="inlineStr">
         <is>
           <t xml:space="preserve">Durability </t>
@@ -6009,6 +6060,8 @@
 View 20 reviews about Compact. 100% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
       <c r="I43" t="inlineStr">
         <is>
           <t xml:space="preserve">Compact </t>
@@ -6052,6 +6105,8 @@
 View 9 reviews about Safety measures. 89% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
       <c r="I44" t="inlineStr">
         <is>
           <t xml:space="preserve">Safety measures </t>
@@ -6095,6 +6150,8 @@
 View 6 reviews about Odor. 67% of the reviews are negative.</t>
         </is>
       </c>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
       <c r="I45" t="inlineStr">
         <is>
           <t xml:space="preserve">Odor </t>
@@ -6297,6 +6354,8 @@
 View 94 reviews about Well made. 87% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
       <c r="I49" t="inlineStr">
         <is>
           <t xml:space="preserve">Well made </t>
@@ -6340,6 +6399,8 @@
 View 41 reviews about Durability. 61% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
       <c r="I50" t="inlineStr">
         <is>
           <t xml:space="preserve">Durability </t>
@@ -6383,6 +6444,8 @@
 View 25 reviews about Compact. 96% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
       <c r="I51" t="inlineStr">
         <is>
           <t xml:space="preserve">Compact </t>
@@ -6426,6 +6489,8 @@
 View 13 reviews about Unpleasant odor. 76% of the reviews are negative.</t>
         </is>
       </c>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
       <c r="I52" t="inlineStr">
         <is>
           <t xml:space="preserve">Unpleasant odor </t>
@@ -6469,6 +6534,8 @@
 View 3 reviews about Safety measures. 67% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
       <c r="I53" t="inlineStr">
         <is>
           <t xml:space="preserve">Safety measures </t>
@@ -6671,6 +6738,8 @@
 View 101 reviews about Sturdy. 86% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
       <c r="I57" t="inlineStr">
         <is>
           <t xml:space="preserve">Sturdy </t>
@@ -6714,6 +6783,8 @@
 View 84 reviews about Well made. 83% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
       <c r="I58" t="inlineStr">
         <is>
           <t xml:space="preserve">Well made </t>
@@ -6757,6 +6828,8 @@
 View 44 reviews about Durability. 64% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr"/>
       <c r="I59" t="inlineStr">
         <is>
           <t xml:space="preserve">Durability </t>
@@ -6800,6 +6873,8 @@
 View 14 reviews about Odor. 64% of the reviews are negative.</t>
         </is>
       </c>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr"/>
       <c r="I60" t="inlineStr">
         <is>
           <t xml:space="preserve">Odor </t>
@@ -6843,6 +6918,8 @@
 View 4 reviews about Safety measures. 75% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr"/>
       <c r="I61" t="inlineStr">
         <is>
           <t xml:space="preserve">Safety measures </t>
@@ -6992,6 +7069,8 @@
 View 57 reviews about Easy to assemble. 79% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr"/>
       <c r="I64" t="inlineStr">
         <is>
           <t xml:space="preserve">Easy to assemble </t>
@@ -7035,6 +7114,8 @@
 View 32 reviews about Sturdy. 84% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr"/>
       <c r="I65" t="inlineStr">
         <is>
           <t xml:space="preserve">Sturdy </t>
@@ -7078,6 +7159,8 @@
 View 38 reviews about Craftsmanship. 61% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G66" t="inlineStr"/>
+      <c r="H66" t="inlineStr"/>
       <c r="I66" t="inlineStr">
         <is>
           <t xml:space="preserve">Craftsmanship </t>
@@ -7121,6 +7204,8 @@
 View 21 reviews about Durability. 62% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G67" t="inlineStr"/>
+      <c r="H67" t="inlineStr"/>
       <c r="I67" t="inlineStr">
         <is>
           <t xml:space="preserve">Durability </t>
@@ -7164,6 +7249,8 @@
 View 3 reviews about Odor. 67% of the reviews are negative.</t>
         </is>
       </c>
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr"/>
       <c r="I68" t="inlineStr">
         <is>
           <t xml:space="preserve">Odor </t>
@@ -7207,6 +7294,8 @@
 View 1 review about Safety measures. 100% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr"/>
       <c r="I69" t="inlineStr">
         <is>
           <t xml:space="preserve">Safety measures </t>
@@ -7409,6 +7498,8 @@
 View 11 reviews about Comfortable. 100% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G73" t="inlineStr"/>
+      <c r="H73" t="inlineStr"/>
       <c r="I73" t="inlineStr">
         <is>
           <t xml:space="preserve">Comfortable </t>
@@ -7452,6 +7543,8 @@
 View 7 reviews about Support. 100% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G74" t="inlineStr"/>
+      <c r="H74" t="inlineStr"/>
       <c r="I74" t="inlineStr">
         <is>
           <t xml:space="preserve">Support </t>
@@ -7495,6 +7588,8 @@
 View 6 reviews about Noise level. 67% of the reviews are negative.</t>
         </is>
       </c>
+      <c r="G75" t="inlineStr"/>
+      <c r="H75" t="inlineStr"/>
       <c r="I75" t="inlineStr">
         <is>
           <t xml:space="preserve">Noise level </t>
@@ -7697,6 +7792,8 @@
 View 53 reviews about Well made. 77% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G79" t="inlineStr"/>
+      <c r="H79" t="inlineStr"/>
       <c r="I79" t="inlineStr">
         <is>
           <t xml:space="preserve">Well made </t>
@@ -7740,6 +7837,8 @@
 View 24 reviews about Durability. 58% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G80" t="inlineStr"/>
+      <c r="H80" t="inlineStr"/>
       <c r="I80" t="inlineStr">
         <is>
           <t xml:space="preserve">Durability </t>
@@ -7783,6 +7882,8 @@
 View 15 reviews about Size. 53% of the reviews are negative.</t>
         </is>
       </c>
+      <c r="G81" t="inlineStr"/>
+      <c r="H81" t="inlineStr"/>
       <c r="I81" t="inlineStr">
         <is>
           <t xml:space="preserve">Size </t>
@@ -7826,6 +7927,8 @@
 View 1 review about Safety measures. 100% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G82" t="inlineStr"/>
+      <c r="H82" t="inlineStr"/>
       <c r="I82" t="inlineStr">
         <is>
           <t xml:space="preserve">Safety measures </t>
@@ -8028,6 +8131,8 @@
 View 50 reviews about Easy to assemble. 98% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G86" t="inlineStr"/>
+      <c r="H86" t="inlineStr"/>
       <c r="I86" t="inlineStr">
         <is>
           <t xml:space="preserve">Easy to assemble </t>
@@ -8071,6 +8176,8 @@
 View 42 reviews about Durable. 86% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G87" t="inlineStr"/>
+      <c r="H87" t="inlineStr"/>
       <c r="I87" t="inlineStr">
         <is>
           <t xml:space="preserve">Durable </t>
@@ -8114,6 +8221,8 @@
 View 6 reviews about Size. 50% of the reviews are negative.</t>
         </is>
       </c>
+      <c r="G88" t="inlineStr"/>
+      <c r="H88" t="inlineStr"/>
       <c r="I88" t="inlineStr">
         <is>
           <t xml:space="preserve">Size </t>
@@ -8316,6 +8425,8 @@
 View 62 reviews about Sturdy. 97% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G92" t="inlineStr"/>
+      <c r="H92" t="inlineStr"/>
       <c r="I92" t="inlineStr">
         <is>
           <t xml:space="preserve">Sturdy </t>
@@ -8359,6 +8470,8 @@
 View 23 reviews about Durability. 52% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G93" t="inlineStr"/>
+      <c r="H93" t="inlineStr"/>
       <c r="I93" t="inlineStr">
         <is>
           <t xml:space="preserve">Durability </t>
@@ -8402,6 +8515,8 @@
 View 10 reviews about Size. 90% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G94" t="inlineStr"/>
+      <c r="H94" t="inlineStr"/>
       <c r="I94" t="inlineStr">
         <is>
           <t xml:space="preserve">Size </t>
@@ -8445,6 +8560,8 @@
 View 9 reviews about Odor. 89% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G95" t="inlineStr"/>
+      <c r="H95" t="inlineStr"/>
       <c r="I95" t="inlineStr">
         <is>
           <t xml:space="preserve">Odor </t>
@@ -8488,6 +8605,8 @@
 View 1 review about Safety measures. 100% of the reviews are negative.</t>
         </is>
       </c>
+      <c r="G96" t="inlineStr"/>
+      <c r="H96" t="inlineStr"/>
       <c r="I96" t="inlineStr">
         <is>
           <t xml:space="preserve">Safety measures </t>
@@ -8690,6 +8809,8 @@
 View 141 reviews about Easy to use. 92% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G100" t="inlineStr"/>
+      <c r="H100" t="inlineStr"/>
       <c r="I100" t="inlineStr">
         <is>
           <t xml:space="preserve">Easy to use </t>
@@ -8733,6 +8854,8 @@
 View 102 reviews about Well made. 98% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G101" t="inlineStr"/>
+      <c r="H101" t="inlineStr"/>
       <c r="I101" t="inlineStr">
         <is>
           <t xml:space="preserve">Well made </t>
@@ -8776,6 +8899,8 @@
 View 90 reviews about Attractive. 99% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G102" t="inlineStr"/>
+      <c r="H102" t="inlineStr"/>
       <c r="I102" t="inlineStr">
         <is>
           <t xml:space="preserve">Attractive </t>
@@ -8819,6 +8944,8 @@
 View 82 reviews about Sturdy. 94% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G103" t="inlineStr"/>
+      <c r="H103" t="inlineStr"/>
       <c r="I103" t="inlineStr">
         <is>
           <t xml:space="preserve">Sturdy </t>
@@ -8862,6 +8989,8 @@
 View 45 reviews about Easy to clean. 100% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G104" t="inlineStr"/>
+      <c r="H104" t="inlineStr"/>
       <c r="I104" t="inlineStr">
         <is>
           <t xml:space="preserve">Easy to clean </t>
@@ -8905,6 +9034,8 @@
 View 31 reviews about Durable. 91% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G105" t="inlineStr"/>
+      <c r="H105" t="inlineStr"/>
       <c r="I105" t="inlineStr">
         <is>
           <t xml:space="preserve">Durable </t>
@@ -8948,6 +9079,8 @@
 View 8 reviews about Ease of putting on/taking off. 100% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G106" t="inlineStr"/>
+      <c r="H106" t="inlineStr"/>
       <c r="I106" t="inlineStr">
         <is>
           <t xml:space="preserve">Ease of putting on/taking off </t>
@@ -8991,6 +9124,8 @@
 View 7 reviews about Safety measures. 100% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G107" t="inlineStr"/>
+      <c r="H107" t="inlineStr"/>
       <c r="I107" t="inlineStr">
         <is>
           <t xml:space="preserve">Safety measures </t>
@@ -9034,6 +9169,8 @@
 View 6 reviews about Instruction quality. 83% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G108" t="inlineStr"/>
+      <c r="H108" t="inlineStr"/>
       <c r="I108" t="inlineStr">
         <is>
           <t xml:space="preserve">Instruction quality </t>
@@ -9077,6 +9214,8 @@
 View 1 review about Storage. 100% of the reviews are positive.</t>
         </is>
       </c>
+      <c r="G109" t="inlineStr"/>
+      <c r="H109" t="inlineStr"/>
       <c r="I109" t="inlineStr">
         <is>
           <t xml:space="preserve">Storage </t>
@@ -9092,367 +9231,6 @@
         <is>
           <t xml:space="preserve"> 100% of the reviews are positive</t>
         </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>url</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>average_total_rating</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>average_reviews</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>sum_positive_percentOfMainFeatures</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>positive_positive_review_percentage</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>log_reviews</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>final_score</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>DaVinci Kalani 4 in 1 Convertible Crib, White</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://www.google.com/shopping/product/15398867985768747083?sca_esv=b22eb09c7ac02542&amp;hl=en-US&amp;psb=1&amp;q=baby+bed&amp;biw=1036&amp;bih=2399&amp;dpr=1.5&amp;prds=eto:15337204680515330759_0,pid:4967143638264096179,rsk:PC_13715925310465574171&amp;sa=X&amp;ved=0ahUKEwjioOHO-72EAxUOLtAFHeq1CR4Q8wII5hM</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1883</v>
-      </c>
-      <c r="E2" t="n">
-        <v>122.1</v>
-      </c>
-      <c r="F2" t="n">
-        <v>90.16666666666667</v>
-      </c>
-      <c r="G2" t="n">
-        <v>7.541152455136308</v>
-      </c>
-      <c r="H2" t="n">
-        <v>4.733112432542714</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Storkcraft - Beckett 3-in-1 Convertible Crib - Natural</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>https://www.google.com/shopping/product/17629737733910496228?sca_esv=b22eb09c7ac02542&amp;hl=en-US&amp;psb=1&amp;q=baby+bed&amp;biw=1036&amp;bih=2399&amp;dpr=1.5&amp;prds=eto:7919916735960715834_0,pid:4701217266289954816,rsk:PC_16960413835488518129&amp;sa=X&amp;ved=0ahUKEwjioOHO-72EAxUOLtAFHeq1CR4Q8wII9xM</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="D3" t="n">
-        <v>647</v>
-      </c>
-      <c r="E3" t="n">
-        <v>123.5</v>
-      </c>
-      <c r="F3" t="n">
-        <v>86.28571428571429</v>
-      </c>
-      <c r="G3" t="n">
-        <v>6.473890696352274</v>
-      </c>
-      <c r="H3" t="n">
-        <v>4.526315067059802</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Storkcraft - Beckett 3-in-1 Convertible Crib - Natural</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>https://www.google.com/shopping/product/17629737733910496228?sca_esv=b22eb09c7ac02542&amp;hl=en-US&amp;psb=1&amp;q=baby+bed&amp;biw=1036&amp;bih=2399&amp;dpr=1.5&amp;prds=eto:7919916735960715834_0,pid:4701217266289954816,rsk:PC_16960413835488518129&amp;sa=X&amp;ved=0ahUKEwjioOHO-72EAxUOLtAFHeq1CR4Q8wIIxBQ</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="D4" t="n">
-        <v>647</v>
-      </c>
-      <c r="E4" t="n">
-        <v>123.5</v>
-      </c>
-      <c r="F4" t="n">
-        <v>86.28571428571429</v>
-      </c>
-      <c r="G4" t="n">
-        <v>6.473890696352274</v>
-      </c>
-      <c r="H4" t="n">
-        <v>4.526315067059802</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Evolur Aurora 5 in 1 Convertible Crib, Blush Pink Pearl</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>https://www.google.com/shopping/product/3740539049733634704?sca_esv=b22eb09c7ac02542&amp;hl=en-US&amp;psb=1&amp;q=baby+bed&amp;biw=1036&amp;bih=2399&amp;dpr=1.5&amp;prds=eto:15127842686872245045_0,pid:13867708756742023682,rsk:PC_18397395286822107211&amp;sa=X&amp;ved=0ahUKEwjioOHO-72EAxUOLtAFHeq1CR4Q8wIImxc</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="D5" t="n">
-        <v>447</v>
-      </c>
-      <c r="E5" t="n">
-        <v>113.7</v>
-      </c>
-      <c r="F5" t="n">
-        <v>95</v>
-      </c>
-      <c r="G5" t="n">
-        <v>6.104793232414985</v>
-      </c>
-      <c r="H5" t="n">
-        <v>4.423536022913661</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Delta Children Deluxe Sweet Beginnings Bassinet, Falling Leaves</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>https://www.google.com/shopping/product/2399006542920773668?sca_esv=b22eb09c7ac02542&amp;hl=en-US&amp;psb=1&amp;q=baby+bed&amp;biw=1036&amp;bih=2399&amp;dpr=1.5&amp;prds=eto:1016384091000436634_0,pid:7295306789158500280,rsk:PC_14716699655969331893&amp;sa=X&amp;ved=0ahUKEwjioOHO-72EAxUOLtAFHeq1CR4Q8wII6xI</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1167</v>
-      </c>
-      <c r="E6" t="n">
-        <v>111.8</v>
-      </c>
-      <c r="F6" t="n">
-        <v>82.54545454545455</v>
-      </c>
-      <c r="G6" t="n">
-        <v>7.063048163388173</v>
-      </c>
-      <c r="H6" t="n">
-        <v>4.419968295456485</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Babyletto Gelato 4-in-1 Convertible Crib with Toddler Bed Conversion Kit Natural Walnut / Gold Feet</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>https://www.google.com/shopping/product/15712459151493487544?sca_esv=b22eb09c7ac02542&amp;hl=en-US&amp;psb=1&amp;q=baby+bed&amp;biw=1036&amp;bih=2399&amp;dpr=1.5&amp;prds=eto:6425704215543786343_0,pid:6680535950108002881,rsk:PC_13925335836916321758&amp;sa=X&amp;ved=0ahUKEwjioOHO-72EAxUOLtAFHeq1CR4Q8wIIpRo</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="D7" t="n">
-        <v>408</v>
-      </c>
-      <c r="E7" t="n">
-        <v>121.1</v>
-      </c>
-      <c r="F7" t="n">
-        <v>85.14285714285714</v>
-      </c>
-      <c r="G7" t="n">
-        <v>6.013715156042802</v>
-      </c>
-      <c r="H7" t="n">
-        <v>4.417349521173927</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Delta Children Folding Portable Mini Crib with Mattress Natural</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>https://www.google.com/shopping/product/332253238461547298?sca_esv=b22eb09c7ac02542&amp;hl=en-US&amp;psb=1&amp;q=baby+bed&amp;biw=1036&amp;bih=2399&amp;dpr=1.5&amp;prds=eto:8449278281958853803_0,pid:17270098338659508229,rsk:PC_2234275959762070381&amp;sa=X&amp;ved=0ahUKEwjioOHO-72EAxUOLtAFHeq1CR4Q8wII_RQ</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="D8" t="n">
-        <v>799</v>
-      </c>
-      <c r="E8" t="n">
-        <v>101.8</v>
-      </c>
-      <c r="F8" t="n">
-        <v>85.28571428571429</v>
-      </c>
-      <c r="G8" t="n">
-        <v>6.684611727667927</v>
-      </c>
-      <c r="H8" t="n">
-        <v>4.27322607987382</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>BabyBjorn Travel Crib Light Bundle Pack - Silver and Fitted Sheet</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>https://www.google.com/shopping/product/1182993104431976221?sca_esv=b22eb09c7ac02542&amp;hl=en-US&amp;psb=1&amp;q=baby+bed&amp;biw=1036&amp;bih=2399&amp;dpr=1.5&amp;prds=pid:11244461425848089325,rsk:PC_9299708097776290589&amp;sa=X&amp;ved=0ahUKEwjioOHO-72EAxUOLtAFHeq1CR4Q8wIIvxw</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="D9" t="n">
-        <v>2463</v>
-      </c>
-      <c r="E9" t="n">
-        <v>62.8</v>
-      </c>
-      <c r="F9" t="n">
-        <v>96.15384615384616</v>
-      </c>
-      <c r="G9" t="n">
-        <v>7.80954132465341</v>
-      </c>
-      <c r="H9" t="n">
-        <v>4.184291497975709</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Sorelle Tuscany 4-in-1 Convertible Crib and Changer Set, Espresso</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>https://www.google.com/shopping/product/2497644496312800615?sca_esv=b22eb09c7ac02542&amp;hl=en-US&amp;psb=1&amp;q=baby+bed&amp;biw=1036&amp;bih=2399&amp;dpr=1.5&amp;prds=eto:11123841242466776316_0,pid:17084826392398359204,rsk:PC_6508002071966735650&amp;sa=X&amp;ved=0ahUKEwjioOHO-72EAxUOLtAFHeq1CR4Q8wII4xY</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="D10" t="n">
-        <v>322</v>
-      </c>
-      <c r="E10" t="n">
-        <v>109.7</v>
-      </c>
-      <c r="F10" t="n">
-        <v>84.16666666666667</v>
-      </c>
-      <c r="G10" t="n">
-        <v>5.777652323222656</v>
-      </c>
-      <c r="H10" t="n">
-        <v>4.163784842849722</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Dream on Me Synergy 5 in 1 Convertible Crib Cool Grey</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>https://www.google.com/shopping/product/12949201208281343090?sca_esv=b22eb09c7ac02542&amp;hl=en-US&amp;psb=1&amp;q=baby+bed&amp;biw=1036&amp;bih=2399&amp;dpr=1.5&amp;prds=eto:16324616383512772686_0,pid:12218184048230842516,rsk:PC_1710838132878600331&amp;sa=X&amp;ved=0ahUKEwjioOHO-72EAxUOLtAFHeq1CR4Q8wII1BM</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="D11" t="n">
-        <v>817</v>
-      </c>
-      <c r="E11" t="n">
-        <v>94.40000000000001</v>
-      </c>
-      <c r="F11" t="n">
-        <v>80.14285714285714</v>
-      </c>
-      <c r="G11" t="n">
-        <v>6.706862336602747</v>
-      </c>
-      <c r="H11" t="n">
-        <v>4.076192701358853</v>
       </c>
     </row>
   </sheetData>

</xml_diff>